<commit_message>
fixed training data error and revamped parser to parse question answer from excel
</commit_message>
<xml_diff>
--- a/tests/testMaterials/CDS_SPARSE_2020_2021.xlsx
+++ b/tests/testMaterials/CDS_SPARSE_2020_2021.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\tests\testMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A64BE0F-DCB2-4C36-A807-A99B343463A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1AC8C7-92A5-4AEF-B782-587BDC1F4FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE1ED6D0-6606-421C-9DB9-B4886BF13D14}"/>
   </bookViews>
   <sheets>
-    <sheet name="General_Enrollment" sheetId="1" r:id="rId1"/>
-    <sheet name="Race_Enrollment" sheetId="2" r:id="rId2"/>
+    <sheet name="Enrollment_General" sheetId="1" r:id="rId1"/>
+    <sheet name="Enrollment_Race" sheetId="2" r:id="rId2"/>
     <sheet name="High School Units" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -3715,11 +3715,16 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
     <col min="14" max="14" width="21.33203125" customWidth="1"/>
   </cols>

</xml_diff>